<commit_message>
formatted all raider_skills csvs and did it for s6 completely
</commit_message>
<xml_diff>
--- a/pypi/prokabaddidata/1_DATA/DATA__Tableau-Data/Defender_Skills/s9_csv/all_defender_skills s9.xlsx
+++ b/pypi/prokabaddidata/1_DATA/DATA__Tableau-Data/Defender_Skills/s9_csv/all_defender_skills s9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annimukh/Documents/acode/ProKabaddi_API/pypi/prokabaddidata/1_DATA/DATA__Tableau-Data/Defender_Skills/s9_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCDBB28-BE48-8C4C-8771-97BCECAC3889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EEEA46-6A70-5C46-9FFD-3A4C5EF231FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="900" windowWidth="41080" windowHeight="24940" xr2:uid="{CFD7F1AD-48C9-43C6-B02C-ECA721CFF2D6}"/>
   </bookViews>
@@ -585,11 +585,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6928DE5-0375-480D-8DF7-F37034F52706}">
   <dimension ref="A1:AT40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AJ23" sqref="AJ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="29" max="29" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>